<commit_message>
sector analysis for other rule sets
</commit_message>
<xml_diff>
--- a/sector_analysis/top_lift_matrix.xlsx
+++ b/sector_analysis/top_lift_matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15840" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Assoc_Rule_Matrix" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="52">
   <si>
     <t>Security</t>
   </si>
@@ -156,6 +156,27 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Same Sector Rules</t>
+  </si>
+  <si>
+    <t>Rules</t>
+  </si>
+  <si>
+    <t>Non-Rules</t>
+  </si>
+  <si>
+    <t>Same Sector Non-Rules</t>
+  </si>
+  <si>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>No Rule</t>
+  </si>
+  <si>
+    <t>Diff Sector</t>
+  </si>
 </sst>
 </file>
 
@@ -215,8 +236,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -240,7 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -250,6 +283,12 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -259,6 +298,12 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -590,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1729,10 +1774,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:U21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3095,6 +3140,9 @@
       </c>
     </row>
     <row r="23" spans="1:21">
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>42</v>
       </c>
@@ -3856,6 +3904,10 @@
       <c r="A33" t="s">
         <v>21</v>
       </c>
+      <c r="B33">
+        <f>COUNTIF(A$4:A$21,A33)</f>
+        <v>8</v>
+      </c>
       <c r="C33" t="s">
         <v>10</v>
       </c>
@@ -3936,79 +3988,83 @@
       <c r="A34" t="s">
         <v>28</v>
       </c>
+      <c r="B34">
+        <f t="shared" ref="B34:B38" si="10">COUNTIF(A$4:A$21,A34)</f>
+        <v>4</v>
+      </c>
       <c r="C34" t="s">
         <v>11</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:U34" si="10">D14*(D$1=$A14)</f>
+        <f t="shared" ref="D34:U34" si="11">D14*(D$1=$A14)</f>
         <v>0</v>
       </c>
       <c r="E34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="H34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4016,79 +4072,83 @@
       <c r="A35" t="s">
         <v>26</v>
       </c>
+      <c r="B35">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
       <c r="C35" t="s">
         <v>12</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:U35" si="11">D15*(D$1=$A15)</f>
+        <f t="shared" ref="D35:U35" si="12">D15*(D$1=$A15)</f>
         <v>0</v>
       </c>
       <c r="E35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="J35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="R35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="S35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="T35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -4096,79 +4156,83 @@
       <c r="A36" t="s">
         <v>29</v>
       </c>
+      <c r="B36">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
       <c r="C36" t="s">
         <v>13</v>
       </c>
       <c r="D36">
-        <f t="shared" ref="D36:U36" si="12">D16*(D$1=$A16)</f>
+        <f t="shared" ref="D36:U36" si="13">D16*(D$1=$A16)</f>
         <v>0</v>
       </c>
       <c r="E36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="G36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="O36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="S36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -4176,79 +4240,83 @@
       <c r="A37" t="s">
         <v>33</v>
       </c>
+      <c r="B37">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:U37" si="13">D17*(D$1=$A17)</f>
+        <f t="shared" ref="D37:U37" si="14">D17*(D$1=$A17)</f>
         <v>1</v>
       </c>
       <c r="E37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="I37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="R37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="T37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="U37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -4256,79 +4324,83 @@
       <c r="A38" t="s">
         <v>37</v>
       </c>
+      <c r="B38">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
       <c r="C38" t="s">
         <v>15</v>
       </c>
       <c r="D38">
-        <f t="shared" ref="D38:U38" si="14">D18*(D$1=$A18)</f>
+        <f t="shared" ref="D38:U38" si="15">D18*(D$1=$A18)</f>
         <v>0</v>
       </c>
       <c r="E38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="G38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="K38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="P38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="S38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="U38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4337,75 +4409,75 @@
         <v>16</v>
       </c>
       <c r="D39">
-        <f t="shared" ref="D39:U39" si="15">D19*(D$1=$A19)</f>
+        <f t="shared" ref="D39:U39" si="16">D19*(D$1=$A19)</f>
         <v>0</v>
       </c>
       <c r="E39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="F39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="G39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="L39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="S39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="T39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -4414,75 +4486,75 @@
         <v>17</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:U40" si="16">D20*(D$1=$A20)</f>
+        <f t="shared" ref="D40:U40" si="17">D20*(D$1=$A20)</f>
         <v>0</v>
       </c>
       <c r="E40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="F40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="G40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="H40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="M40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="P40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="S40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4491,81 +4563,96 @@
         <v>18</v>
       </c>
       <c r="D41">
-        <f t="shared" ref="D41:U41" si="17">D21*(D$1=$A21)</f>
+        <f t="shared" ref="D41:U41" si="18">D21*(D$1=$A21)</f>
         <v>0</v>
       </c>
       <c r="E41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="F41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="G41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="J41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="M41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="R41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="S41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="T41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:21">
+      <c r="C43" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D43" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J43" t="s">
+        <v>49</v>
+      </c>
+      <c r="K43" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:21">
@@ -4573,8 +4660,26 @@
         <v>42</v>
       </c>
       <c r="D44">
-        <f>SUM(D24:U41)</f>
-        <v>16</v>
+        <f>SUM(D24:U41)/2</f>
+        <v>8</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G44">
+        <f>SUM(D48:U65)/2</f>
+        <v>29</v>
+      </c>
+      <c r="I44" t="s">
+        <v>42</v>
+      </c>
+      <c r="J44">
+        <f>D44</f>
+        <v>8</v>
+      </c>
+      <c r="K44">
+        <f>G44</f>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -4582,8 +4687,1456 @@
         <v>43</v>
       </c>
       <c r="D45">
-        <f>SUM(D4:U21)-D44</f>
-        <v>10</v>
+        <f>SUM(D4:U21)/2-D44</f>
+        <v>5</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G45">
+        <f>18*17/2-G44-D44-D45</f>
+        <v>111</v>
+      </c>
+      <c r="I45" t="s">
+        <v>51</v>
+      </c>
+      <c r="J45">
+        <f>D45</f>
+        <v>5</v>
+      </c>
+      <c r="K45">
+        <f>G45</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47" t="s">
+        <v>21</v>
+      </c>
+      <c r="G47" t="s">
+        <v>26</v>
+      </c>
+      <c r="H47" t="s">
+        <v>21</v>
+      </c>
+      <c r="I47" t="s">
+        <v>28</v>
+      </c>
+      <c r="J47" t="s">
+        <v>26</v>
+      </c>
+      <c r="K47" t="s">
+        <v>29</v>
+      </c>
+      <c r="L47" t="s">
+        <v>21</v>
+      </c>
+      <c r="M47" t="s">
+        <v>21</v>
+      </c>
+      <c r="N47" t="s">
+        <v>33</v>
+      </c>
+      <c r="O47" t="s">
+        <v>28</v>
+      </c>
+      <c r="P47" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>21</v>
+      </c>
+      <c r="R47" t="s">
+        <v>28</v>
+      </c>
+      <c r="S47" t="s">
+        <v>37</v>
+      </c>
+      <c r="T47" t="s">
+        <v>26</v>
+      </c>
+      <c r="U47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ref="E48:U63" si="19">(1-E4)*(E$1=$A4)</f>
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U48">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="3:21">
+      <c r="C49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ref="D49:S65" si="20">(1-D5)*(D$1=$A5)</f>
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="3:21">
+      <c r="C50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="3:21">
+      <c r="C51" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="U51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="3:21">
+      <c r="C52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U52">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="3:21">
+      <c r="C53" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T53">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U53">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="3:21">
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="U54">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="3:21">
+      <c r="C55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="3:21">
+      <c r="C56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="R56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="3:21">
+      <c r="C57" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="R57">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S57">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T57">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U57">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="3:21">
+      <c r="C58" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U58">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="3:21">
+      <c r="C59" t="s">
+        <v>28</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T59">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U59">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="3:21">
+      <c r="C60" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U60">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="3:21">
+      <c r="C61" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="Q61">
+        <v>0</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U61">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="3:21">
+      <c r="C62" t="s">
+        <v>28</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R62">
+        <v>0</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U62">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="3:21">
+      <c r="C63" t="s">
+        <v>37</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S63">
+        <v>0</v>
+      </c>
+      <c r="T63">
+        <f t="shared" ref="E63:U65" si="21">(1-T19)*(T$1=$A19)</f>
+        <v>0</v>
+      </c>
+      <c r="U63">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="3:21">
+      <c r="C64" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T64">
+        <v>0</v>
+      </c>
+      <c r="U64">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="3:21">
+      <c r="C65" t="s">
+        <v>28</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R65">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="S65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T65">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="U65">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>